<commit_message>
promises with .then .catch methods
</commit_message>
<xml_diff>
--- a/javascript.xlsx
+++ b/javascript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manji\OneDrive\Desktop\DEV\Javascript revisiting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4837286E-008C-4724-A293-2A425D419CFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1448CBD0-90B1-4EAA-97A5-AC01B503DBF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
   <si>
     <t>Category</t>
   </si>
@@ -181,7 +181,10 @@
     <t>miscellaneous</t>
   </si>
   <si>
-    <t>will return a promise</t>
+    <t xml:space="preserve">check out the code and github please </t>
+  </si>
+  <si>
+    <t>does not suspend the function exe. , return in .then can help to pass the value to next .then method</t>
   </si>
 </sst>
 </file>
@@ -445,8 +448,8 @@
   </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="170" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="93" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -582,12 +585,20 @@
       <c r="C12" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">

</xml_diff>

<commit_message>
hoisting variables and functions
</commit_message>
<xml_diff>
--- a/javascript.xlsx
+++ b/javascript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manji\OneDrive\Desktop\DEV\Javascript revisiting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F764D74-8D7A-4682-9D5D-2E05D2BA2A82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9231B478-08C9-436B-93DF-BD440734861C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t>Category</t>
   </si>
@@ -188,6 +188,15 @@
   </si>
   <si>
     <t>everything is object , __proto__ holds refference to prototype of an object, checkout gitub</t>
+  </si>
+  <si>
+    <t>revisit</t>
+  </si>
+  <si>
+    <t>variable declaration are made undefined, function scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">function defined as variable will always not have hoisting feature and will remain undefined </t>
   </si>
 </sst>
 </file>
@@ -451,8 +460,8 @@
   </sheetPr>
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="91" zoomScaleNormal="156" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="153" zoomScaleNormal="156" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -551,6 +560,9 @@
         <v>11</v>
       </c>
       <c r="C8" s="1"/>
+      <c r="D8" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -568,6 +580,9 @@
         <v>14</v>
       </c>
       <c r="C10" s="1"/>
+      <c r="D10" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -619,6 +634,9 @@
       <c r="C15" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
@@ -627,15 +645,25 @@
       <c r="B16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="C17" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>25</v>
       </c>
@@ -644,13 +672,13 @@
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>28</v>
       </c>
@@ -659,13 +687,13 @@
       </c>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>31</v>
       </c>
@@ -674,13 +702,13 @@
       </c>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -689,12 +717,12 @@
       </c>
       <c r="C24" s="1"/>
     </row>
-    <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -705,7 +733,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -716,12 +744,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>50</v>
       </c>

</xml_diff>